<commit_message>
pushing code to branch
</commit_message>
<xml_diff>
--- a/ExternalFiles/ExcelRead.xlsx
+++ b/ExternalFiles/ExcelRead.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15750" windowHeight="6540"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16140" windowHeight="4395"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>UserName</t>
   </si>
@@ -56,13 +56,40 @@
   </si>
   <si>
     <t>MobileNo</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>gabc@gmail.com</t>
+  </si>
+  <si>
+    <t>Gauravnaukri@11</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>nabc@gmail.com</t>
+  </si>
+  <si>
+    <t>Nehanaukri@11</t>
+  </si>
+  <si>
+    <t>Saurabh</t>
+  </si>
+  <si>
+    <t>sabc@gmail.com</t>
+  </si>
+  <si>
+    <t>Saurabhnaukri@11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +97,14 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,14 +130,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,7 +464,57 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>9911227788</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>9966332255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>9874563211</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>